<commit_message>
gth and rgth file
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/demodata.xlsx
+++ b/src/test/java/TestData/demodata.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
     <sheet name="dpc" sheetId="2" r:id="rId2"/>
-    <sheet name="demo" sheetId="3" r:id="rId3"/>
+    <sheet name="rgth" sheetId="3" r:id="rId3"/>
+    <sheet name="pgth" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>TestCases</t>
   </si>
@@ -87,15 +88,6 @@
     <t>Describe the nature of the business, including its address and country and other details to help identify the company</t>
   </si>
   <si>
-    <t>vendorsupplier</t>
-  </si>
-  <si>
-    <t>Describe nature</t>
-  </si>
-  <si>
-    <t>relation</t>
-  </si>
-  <si>
     <t>relationship</t>
   </si>
   <si>
@@ -105,17 +97,121 @@
     <t xml:space="preserve">Additional information </t>
   </si>
   <si>
-    <t>COI_Automation3</t>
+    <t>ak@gmail.com</t>
+  </si>
+  <si>
+    <t>competitor</t>
+  </si>
+  <si>
+    <t>company competes</t>
+  </si>
+  <si>
+    <t>Employer</t>
+  </si>
+  <si>
+    <t>Offical_Position</t>
+  </si>
+  <si>
+    <t>Full_Name</t>
+  </si>
+  <si>
+    <t>Request_Name</t>
+  </si>
+  <si>
+    <t>email_address</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Business_Purpose</t>
+  </si>
+  <si>
+    <t>Monetary_Value</t>
+  </si>
+  <si>
+    <t>Shreya</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Details about the gift, travel or hospitality</t>
+  </si>
+  <si>
+    <t>Business Purpose or Rationale.</t>
+  </si>
+  <si>
+    <t>RequestName</t>
+  </si>
+  <si>
+    <t>Describe the gift</t>
+  </si>
+  <si>
+    <t>hospitality in detail, including the business purpose or rationale</t>
+  </si>
+  <si>
+    <t>Additional Information</t>
+  </si>
+  <si>
+    <t>upload any additional files to support your approval request (optional).</t>
+  </si>
+  <si>
+    <t>Sort Description</t>
+  </si>
+  <si>
+    <t>Category Entertainment</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>akshay</t>
+  </si>
+  <si>
+    <t>kapil</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>COI_Auto</t>
+  </si>
+  <si>
+    <t>Receive Gift Auto</t>
+  </si>
+  <si>
+    <t>Provide Gift Auto</t>
+  </si>
+  <si>
+    <t>aagg@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -138,16 +234,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -537,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,20 +659,20 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>22</v>
@@ -581,35 +680,220 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add org and individuals script
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/demodata.xlsx
+++ b/src/test/java/TestData/demodata.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="13335" windowHeight="3705" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13605" windowHeight="3930" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
     <sheet name="dpc" sheetId="2" r:id="rId2"/>
-    <sheet name="rgth" sheetId="3" r:id="rId3"/>
-    <sheet name="pgth" sheetId="4" r:id="rId4"/>
+    <sheet name="EXF" sheetId="5" r:id="rId3"/>
+    <sheet name="pgthr" sheetId="6" r:id="rId4"/>
+    <sheet name="gthr" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:J11"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="79">
   <si>
     <t>TestCases</t>
   </si>
@@ -82,9 +84,6 @@
     <t>Request Name</t>
   </si>
   <si>
-    <t>Akshay</t>
-  </si>
-  <si>
     <t>Describe the nature of the business, including its address and country and other details to help identify the company</t>
   </si>
   <si>
@@ -109,18 +108,12 @@
     <t>Employer</t>
   </si>
   <si>
-    <t>Offical_Position</t>
-  </si>
-  <si>
     <t>Full_Name</t>
   </si>
   <si>
     <t>Request_Name</t>
   </si>
   <si>
-    <t>email_address</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -133,60 +126,21 @@
     <t>QA</t>
   </si>
   <si>
-    <t>Details about the gift, travel or hospitality</t>
-  </si>
-  <si>
-    <t>Business Purpose or Rationale.</t>
-  </si>
-  <si>
     <t>RequestName</t>
   </si>
   <si>
     <t>Describe the gift</t>
   </si>
   <si>
-    <t>hospitality in detail, including the business purpose or rationale</t>
-  </si>
-  <si>
     <t>Additional Information</t>
   </si>
   <si>
-    <t>upload any additional files to support your approval request (optional).</t>
-  </si>
-  <si>
     <t>Sort Description</t>
   </si>
   <si>
-    <t>Category Entertainment</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
     <t>FullName</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Tester</t>
-  </si>
-  <si>
-    <t>akshay</t>
-  </si>
-  <si>
-    <t>kapil</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Receive Gift Auto</t>
-  </si>
-  <si>
-    <t>Provide Gift Auto</t>
-  </si>
-  <si>
     <t>COI_Competitors</t>
   </si>
   <si>
@@ -205,10 +159,103 @@
     <t>RelationshipCustomer</t>
   </si>
   <si>
-    <t>aagg5@gmail.com</t>
-  </si>
-  <si>
-    <t>Viktor</t>
+    <t>Recipient Name</t>
+  </si>
+  <si>
+    <t>External Funding</t>
+  </si>
+  <si>
+    <t>Funding Request Name</t>
+  </si>
+  <si>
+    <t>Provide External Funding Request</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Mission Description</t>
+  </si>
+  <si>
+    <t>Detailed description of the mission of the organization and the types of medical,</t>
+  </si>
+  <si>
+    <t>Detail Organization</t>
+  </si>
+  <si>
+    <t>Detail how the organization was identified:</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Funding Details</t>
+  </si>
+  <si>
+    <t>Describe the external funding in detail, including how it will support legitimate medical, educational, charitable or social welfare activities that are aligned with the company's interests:</t>
+  </si>
+  <si>
+    <t>EmployerName</t>
+  </si>
+  <si>
+    <t>AddFullName</t>
+  </si>
+  <si>
+    <t>AddOfficialPosition</t>
+  </si>
+  <si>
+    <t>Provide Gift</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>Default Amount</t>
+  </si>
+  <si>
+    <t>Official Name</t>
+  </si>
+  <si>
+    <t>AddOrganization</t>
+  </si>
+  <si>
+    <t>IndividualFullName</t>
+  </si>
+  <si>
+    <t>IndividualOfficialPosition</t>
+  </si>
+  <si>
+    <t>OrganizationOfficialName</t>
+  </si>
+  <si>
+    <t>Received Gift Auto</t>
+  </si>
+  <si>
+    <t>AKR1</t>
+  </si>
+  <si>
+    <t>AK1</t>
+  </si>
+  <si>
+    <t>Mukul1</t>
+  </si>
+  <si>
+    <t>KapilJain1</t>
+  </si>
+  <si>
+    <t>AkshayRajput1</t>
+  </si>
+  <si>
+    <t>ViktorS1</t>
   </si>
 </sst>
 </file>
@@ -649,10 +696,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,63 +721,71 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -743,16 +798,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -765,88 +820,77 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
+        <v>50</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
+        <v>55</v>
+      </c>
+      <c r="B7">
+        <v>500</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9">
-        <v>500</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -859,80 +903,184 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="2">
-        <v>500</v>
+        <v>66</v>
+      </c>
+      <c r="B6">
+        <v>2000</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
         <v>62</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10">
+        <v>500</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>